<commit_message>
meets thru December 2019
</commit_message>
<xml_diff>
--- a/USASwimming/Times For Declan Keane.xlsx
+++ b/USASwimming/Times For Declan Keane.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="44">
   <si>
     <t>Event</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>11/9/2019</t>
+  </si>
+  <si>
+    <t>41.19r</t>
   </si>
   <si>
     <t>100 FR</t>
@@ -511,7 +514,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J36"/>
+  <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -599,19 +602,19 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="3">
-        <v>33.501084259259258</v>
-      </c>
-      <c r="C3" s="3">
-        <v>33.501084259259258</v>
+      <c r="C3" s="2">
+        <v>36557.50047673611</v>
       </c>
       <c r="D3">
         <v>8</v>
       </c>
       <c r="E3">
-        <v>81</v>
+        <v>162</v>
       </c>
       <c r="F3" t="s">
         <v>11</v>
@@ -626,24 +629,24 @@
         <v>14</v>
       </c>
       <c r="J3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="2">
-        <v>33.500580324074072</v>
-      </c>
-      <c r="C4" s="2">
-        <v>36557.500580324071</v>
+        <v>17</v>
+      </c>
+      <c r="B4" s="3">
+        <v>33.501084259259258</v>
+      </c>
+      <c r="C4" s="3">
+        <v>33.501084259259258</v>
       </c>
       <c r="D4">
         <v>8</v>
       </c>
       <c r="E4">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="F4" t="s">
         <v>11</v>
@@ -658,7 +661,7 @@
         <v>14</v>
       </c>
       <c r="J4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -666,16 +669,16 @@
         <v>19</v>
       </c>
       <c r="B5" s="2">
-        <v>33.50064861111111</v>
+        <v>33.500580324074072</v>
       </c>
       <c r="C5" s="2">
-        <v>36557.500648611109</v>
+        <v>36557.500580324071</v>
       </c>
       <c r="D5">
         <v>8</v>
       </c>
       <c r="E5">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="F5" t="s">
         <v>11</v>
@@ -690,24 +693,24 @@
         <v>14</v>
       </c>
       <c r="J5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="3">
-        <v>33.501423148148149</v>
-      </c>
-      <c r="C6" s="3">
-        <v>33.501423148148149</v>
+      <c r="B6" s="2">
+        <v>33.50064861111111</v>
+      </c>
+      <c r="C6" s="2">
+        <v>36557.500648611109</v>
       </c>
       <c r="D6">
         <v>8</v>
       </c>
       <c r="E6">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F6" t="s">
         <v>11</v>
@@ -722,30 +725,30 @@
         <v>14</v>
       </c>
       <c r="J6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="2">
-        <v>33.50059675925926</v>
-      </c>
-      <c r="C7" s="2">
-        <v>36557.500596759259</v>
+        <v>21</v>
+      </c>
+      <c r="B7" s="3">
+        <v>33.501423148148149</v>
+      </c>
+      <c r="C7" s="3">
+        <v>33.501423148148149</v>
       </c>
       <c r="D7">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E7">
-        <v>23</v>
+        <v>88</v>
       </c>
       <c r="F7" t="s">
         <v>11</v>
       </c>
       <c r="G7" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="H7" t="s">
         <v>13</v>
@@ -754,7 +757,7 @@
         <v>14</v>
       </c>
       <c r="J7" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -762,31 +765,31 @@
         <v>10</v>
       </c>
       <c r="B8" s="2">
-        <v>33.500601620370368</v>
+        <v>33.50059675925926</v>
       </c>
       <c r="C8" s="2">
-        <v>36557.50060162037</v>
+        <v>36557.500596759259</v>
       </c>
       <c r="D8">
         <v>7</v>
       </c>
       <c r="E8">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="F8" t="s">
         <v>11</v>
       </c>
       <c r="G8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8" t="s">
         <v>23</v>
-      </c>
-      <c r="H8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I8" t="s">
-        <v>14</v>
-      </c>
-      <c r="J8" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -794,31 +797,31 @@
         <v>10</v>
       </c>
       <c r="B9" s="2">
-        <v>33.500634606481484</v>
+        <v>33.500601620370368</v>
       </c>
       <c r="C9" s="2">
-        <v>36557.500634606484</v>
+        <v>36557.50060162037</v>
       </c>
       <c r="D9">
         <v>7</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F9" t="s">
         <v>11</v>
       </c>
       <c r="G9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J9" t="s">
         <v>25</v>
-      </c>
-      <c r="H9" t="s">
-        <v>13</v>
-      </c>
-      <c r="I9" t="s">
-        <v>14</v>
-      </c>
-      <c r="J9" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -826,10 +829,10 @@
         <v>10</v>
       </c>
       <c r="B10" s="2">
-        <v>33.500646064814816</v>
+        <v>33.500634606481484</v>
       </c>
       <c r="C10" s="2">
-        <v>36557.500646064815</v>
+        <v>36557.500634606484</v>
       </c>
       <c r="D10">
         <v>7</v>
@@ -841,16 +844,16 @@
         <v>11</v>
       </c>
       <c r="G10" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10" t="s">
+        <v>14</v>
+      </c>
+      <c r="J10" t="s">
         <v>27</v>
-      </c>
-      <c r="H10" t="s">
-        <v>13</v>
-      </c>
-      <c r="I10" t="s">
-        <v>14</v>
-      </c>
-      <c r="J10" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -858,10 +861,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="2">
-        <v>33.500666550925928</v>
+        <v>33.500646064814816</v>
       </c>
       <c r="C11" s="2">
-        <v>36557.500666550928</v>
+        <v>36557.500646064815</v>
       </c>
       <c r="D11">
         <v>7</v>
@@ -873,27 +876,27 @@
         <v>11</v>
       </c>
       <c r="G11" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11" t="s">
+        <v>13</v>
+      </c>
+      <c r="I11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J11" t="s">
         <v>29</v>
-      </c>
-      <c r="H11" t="s">
-        <v>13</v>
-      </c>
-      <c r="I11" t="s">
-        <v>14</v>
-      </c>
-      <c r="J11" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="3">
-        <v>33.500710185185184</v>
-      </c>
-      <c r="C12" s="3">
-        <v>33.500710185185184</v>
+      <c r="B12" s="2">
+        <v>33.500666550925928</v>
+      </c>
+      <c r="C12" s="2">
+        <v>36557.500666550928</v>
       </c>
       <c r="D12">
         <v>7</v>
@@ -905,16 +908,16 @@
         <v>11</v>
       </c>
       <c r="G12" t="s">
+        <v>30</v>
+      </c>
+      <c r="H12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I12" t="s">
+        <v>14</v>
+      </c>
+      <c r="J12" t="s">
         <v>31</v>
-      </c>
-      <c r="H12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I12" t="s">
-        <v>14</v>
-      </c>
-      <c r="J12" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -922,13 +925,13 @@
         <v>10</v>
       </c>
       <c r="B13" s="3">
-        <v>33.500829629629628</v>
+        <v>33.500710185185184</v>
       </c>
       <c r="C13" s="3">
-        <v>33.500829629629628</v>
+        <v>33.500710185185184</v>
       </c>
       <c r="D13">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E13">
         <v>1</v>
@@ -937,16 +940,16 @@
         <v>11</v>
       </c>
       <c r="G13" t="s">
+        <v>32</v>
+      </c>
+      <c r="H13" t="s">
+        <v>13</v>
+      </c>
+      <c r="I13" t="s">
+        <v>14</v>
+      </c>
+      <c r="J13" t="s">
         <v>33</v>
-      </c>
-      <c r="H13" t="s">
-        <v>13</v>
-      </c>
-      <c r="I13" t="s">
-        <v>14</v>
-      </c>
-      <c r="J13" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -954,10 +957,10 @@
         <v>10</v>
       </c>
       <c r="B14" s="3">
-        <v>33.50096099537037</v>
+        <v>33.500829629629628</v>
       </c>
       <c r="C14" s="3">
-        <v>33.50096099537037</v>
+        <v>33.500829629629628</v>
       </c>
       <c r="D14">
         <v>6</v>
@@ -969,30 +972,30 @@
         <v>11</v>
       </c>
       <c r="G14" t="s">
+        <v>34</v>
+      </c>
+      <c r="H14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I14" t="s">
+        <v>14</v>
+      </c>
+      <c r="J14" t="s">
         <v>35</v>
-      </c>
-      <c r="H14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I14" t="s">
-        <v>14</v>
-      </c>
-      <c r="J14" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B15" s="3">
-        <v>33.501335185185184</v>
+        <v>33.50096099537037</v>
       </c>
       <c r="C15" s="3">
-        <v>33.501335185185184</v>
+        <v>33.50096099537037</v>
       </c>
       <c r="D15">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -1001,7 +1004,7 @@
         <v>11</v>
       </c>
       <c r="G15" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="H15" t="s">
         <v>13</v>
@@ -1010,18 +1013,18 @@
         <v>14</v>
       </c>
       <c r="J15" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B16" s="3">
-        <v>33.501385416666665</v>
+        <v>33.501335185185184</v>
       </c>
       <c r="C16" s="3">
-        <v>33.501385416666665</v>
+        <v>33.501335185185184</v>
       </c>
       <c r="D16">
         <v>7</v>
@@ -1033,7 +1036,7 @@
         <v>11</v>
       </c>
       <c r="G16" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="H16" t="s">
         <v>13</v>
@@ -1042,18 +1045,18 @@
         <v>14</v>
       </c>
       <c r="J16" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B17" s="3">
-        <v>33.501445717592595</v>
+        <v>33.501385416666665</v>
       </c>
       <c r="C17" s="3">
-        <v>33.501445717592595</v>
+        <v>33.501385416666665</v>
       </c>
       <c r="D17">
         <v>7</v>
@@ -1065,7 +1068,7 @@
         <v>11</v>
       </c>
       <c r="G17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H17" t="s">
         <v>13</v>
@@ -1079,13 +1082,13 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B18" s="3">
-        <v>33.501526388888891</v>
+        <v>33.501445717592595</v>
       </c>
       <c r="C18" s="3">
-        <v>33.501526388888891</v>
+        <v>33.501445717592595</v>
       </c>
       <c r="D18">
         <v>7</v>
@@ -1097,7 +1100,7 @@
         <v>11</v>
       </c>
       <c r="G18" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="H18" t="s">
         <v>13</v>
@@ -1106,18 +1109,18 @@
         <v>14</v>
       </c>
       <c r="J18" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B19" s="3">
-        <v>33.501561805555554</v>
+        <v>33.501526388888891</v>
       </c>
       <c r="C19" s="3">
-        <v>33.501561805555554</v>
+        <v>33.501526388888891</v>
       </c>
       <c r="D19">
         <v>7</v>
@@ -1129,7 +1132,7 @@
         <v>11</v>
       </c>
       <c r="G19" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="H19" t="s">
         <v>13</v>
@@ -1138,30 +1141,30 @@
         <v>14</v>
       </c>
       <c r="J19" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="2">
-        <v>33.500669212962961</v>
-      </c>
-      <c r="C20" s="2">
-        <v>36557.500669212961</v>
+        <v>17</v>
+      </c>
+      <c r="B20" s="3">
+        <v>33.501561805555554</v>
+      </c>
+      <c r="C20" s="3">
+        <v>33.501561805555554</v>
       </c>
       <c r="D20">
         <v>7</v>
       </c>
       <c r="E20">
-        <v>62</v>
+        <v>1</v>
       </c>
       <c r="F20" t="s">
         <v>11</v>
       </c>
       <c r="G20" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="H20" t="s">
         <v>13</v>
@@ -1170,62 +1173,62 @@
         <v>14</v>
       </c>
       <c r="J20" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B21" s="2">
-        <v>33.500685995370368</v>
+        <v>33.500669212962961</v>
       </c>
       <c r="C21" s="2">
-        <v>36557.500685995372</v>
+        <v>36557.500669212961</v>
       </c>
       <c r="D21">
         <v>7</v>
       </c>
       <c r="E21">
-        <v>33</v>
+        <v>62</v>
       </c>
       <c r="F21" t="s">
         <v>11</v>
       </c>
       <c r="G21" t="s">
+        <v>22</v>
+      </c>
+      <c r="H21" t="s">
+        <v>13</v>
+      </c>
+      <c r="I21" t="s">
+        <v>14</v>
+      </c>
+      <c r="J21" t="s">
         <v>23</v>
-      </c>
-      <c r="H21" t="s">
-        <v>13</v>
-      </c>
-      <c r="I21" t="s">
-        <v>14</v>
-      </c>
-      <c r="J21" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B22" s="2">
-        <v>33.500689583333333</v>
+        <v>33.500685995370368</v>
       </c>
       <c r="C22" s="2">
-        <v>36557.500689583336</v>
+        <v>36557.500685995372</v>
       </c>
       <c r="D22">
         <v>7</v>
       </c>
       <c r="E22">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="F22" t="s">
         <v>11</v>
       </c>
       <c r="G22" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H22" t="s">
         <v>13</v>
@@ -1234,30 +1237,30 @@
         <v>14</v>
       </c>
       <c r="J22" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>18</v>
-      </c>
-      <c r="B23" s="3">
-        <v>33.500701736111111</v>
-      </c>
-      <c r="C23" s="3">
-        <v>33.500701736111111</v>
+        <v>19</v>
+      </c>
+      <c r="B23" s="2">
+        <v>33.500689583333333</v>
+      </c>
+      <c r="C23" s="2">
+        <v>36557.500689583336</v>
       </c>
       <c r="D23">
         <v>7</v>
       </c>
       <c r="E23">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="F23" t="s">
         <v>11</v>
       </c>
       <c r="G23" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H23" t="s">
         <v>13</v>
@@ -1266,30 +1269,30 @@
         <v>14</v>
       </c>
       <c r="J23" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B24" s="3">
-        <v>33.500738310185184</v>
+        <v>33.500701736111111</v>
       </c>
       <c r="C24" s="3">
-        <v>33.500738310185184</v>
+        <v>33.500701736111111</v>
       </c>
       <c r="D24">
         <v>7</v>
       </c>
       <c r="E24">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F24" t="s">
         <v>11</v>
       </c>
       <c r="G24" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="H24" t="s">
         <v>13</v>
@@ -1298,18 +1301,18 @@
         <v>14</v>
       </c>
       <c r="J24" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B25" s="3">
-        <v>33.500761458333336</v>
+        <v>33.500738310185184</v>
       </c>
       <c r="C25" s="3">
-        <v>33.500761458333336</v>
+        <v>33.500738310185184</v>
       </c>
       <c r="D25">
         <v>7</v>
@@ -1321,7 +1324,7 @@
         <v>11</v>
       </c>
       <c r="G25" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="H25" t="s">
         <v>13</v>
@@ -1330,21 +1333,21 @@
         <v>14</v>
       </c>
       <c r="J25" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B26" s="3">
-        <v>33.500886805555552</v>
+        <v>33.500761458333336</v>
       </c>
       <c r="C26" s="3">
-        <v>33.500886805555552</v>
+        <v>33.500761458333336</v>
       </c>
       <c r="D26">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E26">
         <v>1</v>
@@ -1353,7 +1356,7 @@
         <v>11</v>
       </c>
       <c r="G26" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H26" t="s">
         <v>13</v>
@@ -1362,18 +1365,18 @@
         <v>14</v>
       </c>
       <c r="J26" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B27" s="3">
-        <v>33.501081134259259</v>
+        <v>33.500886805555552</v>
       </c>
       <c r="C27" s="3">
-        <v>33.501081134259259</v>
+        <v>33.500886805555552</v>
       </c>
       <c r="D27">
         <v>6</v>
@@ -1385,7 +1388,7 @@
         <v>11</v>
       </c>
       <c r="G27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H27" t="s">
         <v>13</v>
@@ -1394,21 +1397,21 @@
         <v>14</v>
       </c>
       <c r="J27" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="B28" s="3">
-        <v>33.501675810185183</v>
+        <v>33.501081134259259</v>
       </c>
       <c r="C28" s="3">
-        <v>33.501675810185183</v>
+        <v>33.501081134259259</v>
       </c>
       <c r="D28">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E28">
         <v>1</v>
@@ -1417,7 +1420,7 @@
         <v>11</v>
       </c>
       <c r="G28" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="H28" t="s">
         <v>13</v>
@@ -1426,30 +1429,30 @@
         <v>14</v>
       </c>
       <c r="J28" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="B29" s="3">
-        <v>33.500778356481483</v>
+        <v>33.501675810185183</v>
       </c>
       <c r="C29" s="3">
-        <v>33.500778356481483</v>
+        <v>33.501675810185183</v>
       </c>
       <c r="D29">
         <v>7</v>
       </c>
       <c r="E29">
-        <v>41</v>
+        <v>1</v>
       </c>
       <c r="F29" t="s">
         <v>11</v>
       </c>
       <c r="G29" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="H29" t="s">
         <v>13</v>
@@ -1458,30 +1461,30 @@
         <v>14</v>
       </c>
       <c r="J29" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B30" s="3">
-        <v>33.500794675925924</v>
+        <v>33.500778356481483</v>
       </c>
       <c r="C30" s="3">
-        <v>33.500794675925924</v>
+        <v>33.500778356481483</v>
       </c>
       <c r="D30">
         <v>7</v>
       </c>
       <c r="E30">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="F30" t="s">
         <v>11</v>
       </c>
       <c r="G30" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="H30" t="s">
         <v>13</v>
@@ -1490,30 +1493,30 @@
         <v>14</v>
       </c>
       <c r="J30" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>20</v>
+      </c>
+      <c r="B31" s="3">
+        <v>33.500794675925924</v>
+      </c>
+      <c r="C31" s="3">
+        <v>33.500794675925924</v>
+      </c>
+      <c r="D31">
+        <v>7</v>
+      </c>
+      <c r="E31">
         <v>19</v>
       </c>
-      <c r="B31" s="3">
-        <v>33.500798958333334</v>
-      </c>
-      <c r="C31" s="3">
-        <v>33.500798958333334</v>
-      </c>
-      <c r="D31">
-        <v>7</v>
-      </c>
-      <c r="E31">
-        <v>14</v>
-      </c>
       <c r="F31" t="s">
         <v>11</v>
       </c>
       <c r="G31" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="H31" t="s">
         <v>13</v>
@@ -1522,30 +1525,30 @@
         <v>14</v>
       </c>
       <c r="J31" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B32" s="3">
-        <v>33.500832754629627</v>
+        <v>33.500798958333334</v>
       </c>
       <c r="C32" s="3">
-        <v>33.500832754629627</v>
+        <v>33.500798958333334</v>
       </c>
       <c r="D32">
         <v>7</v>
       </c>
       <c r="E32">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F32" t="s">
         <v>11</v>
       </c>
       <c r="G32" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H32" t="s">
         <v>13</v>
@@ -1554,18 +1557,18 @@
         <v>14</v>
       </c>
       <c r="J32" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B33" s="3">
-        <v>33.500835069444442</v>
+        <v>33.500832754629627</v>
       </c>
       <c r="C33" s="3">
-        <v>33.500835069444442</v>
+        <v>33.500832754629627</v>
       </c>
       <c r="D33">
         <v>7</v>
@@ -1577,7 +1580,7 @@
         <v>11</v>
       </c>
       <c r="G33" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="H33" t="s">
         <v>13</v>
@@ -1586,18 +1589,18 @@
         <v>14</v>
       </c>
       <c r="J33" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B34" s="3">
-        <v>33.500861574074072</v>
+        <v>33.500835069444442</v>
       </c>
       <c r="C34" s="3">
-        <v>33.500861574074072</v>
+        <v>33.500835069444442</v>
       </c>
       <c r="D34">
         <v>7</v>
@@ -1609,7 +1612,7 @@
         <v>11</v>
       </c>
       <c r="G34" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="H34" t="s">
         <v>13</v>
@@ -1618,7 +1621,7 @@
         <v>14</v>
       </c>
       <c r="J34" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -1626,22 +1629,22 @@
         <v>20</v>
       </c>
       <c r="B35" s="3">
-        <v>33.501679976851854</v>
+        <v>33.500861574074072</v>
       </c>
       <c r="C35" s="3">
-        <v>33.501679976851854</v>
+        <v>33.500861574074072</v>
       </c>
       <c r="D35">
         <v>7</v>
       </c>
       <c r="E35">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="F35" t="s">
         <v>11</v>
       </c>
       <c r="G35" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H35" t="s">
         <v>13</v>
@@ -1650,39 +1653,71 @@
         <v>14</v>
       </c>
       <c r="J35" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B36" s="3">
+        <v>33.501679976851854</v>
+      </c>
+      <c r="C36" s="3">
+        <v>33.501679976851854</v>
+      </c>
+      <c r="D36">
+        <v>7</v>
+      </c>
+      <c r="E36">
+        <v>57</v>
+      </c>
+      <c r="F36" t="s">
+        <v>11</v>
+      </c>
+      <c r="G36" t="s">
+        <v>28</v>
+      </c>
+      <c r="H36" t="s">
+        <v>13</v>
+      </c>
+      <c r="I36" t="s">
+        <v>14</v>
+      </c>
+      <c r="J36" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>21</v>
+      </c>
+      <c r="B37" s="3">
         <v>33.501843055555554</v>
       </c>
-      <c r="C36" s="3">
+      <c r="C37" s="3">
         <v>33.501843055555554</v>
       </c>
-      <c r="D36">
-        <v>7</v>
-      </c>
-      <c r="E36">
-        <v>1</v>
-      </c>
-      <c r="F36" t="s">
-        <v>11</v>
-      </c>
-      <c r="G36" t="s">
-        <v>29</v>
-      </c>
-      <c r="H36" t="s">
-        <v>13</v>
-      </c>
-      <c r="I36" t="s">
-        <v>14</v>
-      </c>
-      <c r="J36" t="s">
+      <c r="D37">
+        <v>7</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37" t="s">
+        <v>11</v>
+      </c>
+      <c r="G37" t="s">
         <v>30</v>
+      </c>
+      <c r="H37" t="s">
+        <v>13</v>
+      </c>
+      <c r="I37" t="s">
+        <v>14</v>
+      </c>
+      <c r="J37" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>